<commit_message>
complete task 1b sentence generation
</commit_message>
<xml_diff>
--- a/data/sample_grammar_rules.xlsx
+++ b/data/sample_grammar_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUT\241\CO3085_NLP\assignment1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489CC0E1-BEC0-4403-A99B-DD14054E1C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6E44FD-BC1A-404E-95D7-E8BC65205D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A2:A49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,243 +514,243 @@
     <col min="1" max="1" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>